<commit_message>
Fix some issues with the 12x8 block
</commit_message>
<xml_diff>
--- a/docs/Blocks.xlsx
+++ b/docs/Blocks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmnielsen/BW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmnielsen/BW/Stardust/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD3DF20-8A0F-6D43-A5B7-4244DFC2B8E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAA1334-F1C6-5C4C-B9C6-DAEF44385E2D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="460" windowWidth="31260" windowHeight="20540" activeTab="2" xr2:uid="{A8F001C3-164F-CB44-AE85-D1EDAAFCF585}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Normal Blocks" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="54">
   <si>
     <t>L</t>
   </si>
@@ -193,6 +192,9 @@
   </si>
   <si>
     <t>2 Pylons</t>
+  </si>
+  <si>
+    <t>* Left or right side can be on map edge, as long as we put pylons in the middle along the edge</t>
   </si>
 </sst>
 </file>
@@ -689,9 +691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0F9ED0-5771-1442-9F18-E1B361EBF084}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2902,8 +2902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90DFA3C2-026B-9A43-980D-E8D28F7CC247}">
   <dimension ref="B1:AG183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="D179" sqref="D179"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4366,7 +4366,7 @@
         <v>0</v>
       </c>
       <c r="O41" s="10" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">
@@ -4475,17 +4475,16 @@
         <v>1</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M44" s="3" t="s">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M44" s="2"/>
+      <c r="N44" s="5"/>
       <c r="O44" s="5"/>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
@@ -4514,17 +4513,16 @@
         <v>1</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K45" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="L45" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M45" s="9" t="s">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L45" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M45" s="8"/>
+      <c r="N45" s="5"/>
       <c r="O45" s="5"/>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add additional start blocks to handle all COG maps
</commit_message>
<xml_diff>
--- a/docs/Blocks.xlsx
+++ b/docs/Blocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmnielsen/BW/Stardust/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAA1334-F1C6-5C4C-B9C6-DAEF44385E2D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934A564F-E2AE-C74B-94A3-0C953A3AF092}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="460" windowWidth="31260" windowHeight="20540" activeTab="2" xr2:uid="{A8F001C3-164F-CB44-AE85-D1EDAAFCF585}"/>
+    <workbookView xWindow="1120" yWindow="460" windowWidth="31260" windowHeight="20540" activeTab="1" xr2:uid="{A8F001C3-164F-CB44-AE85-D1EDAAFCF585}"/>
   </bookViews>
   <sheets>
     <sheet name="Power" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="58">
   <si>
     <t>L</t>
   </si>
@@ -195,6 +195,18 @@
   </si>
   <si>
     <t>* Left or right side can be on map edge, as long as we put pylons in the middle along the edge</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Above-left of nexus, horizontal</t>
+  </si>
+  <si>
+    <t>Left of nexus, compact horizontal</t>
+  </si>
+  <si>
+    <t>Right of nexus, vertical</t>
   </si>
 </sst>
 </file>
@@ -689,9 +701,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0F9ED0-5771-1442-9F18-E1B361EBF084}">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:AO38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1078,7 +1092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1131,7 +1145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1148,7 +1162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1159,7 +1173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
@@ -1182,7 +1196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>2</v>
       </c>
@@ -1206,7 +1220,7 @@
       </c>
       <c r="S22" s="5"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>2</v>
       </c>
@@ -1234,7 +1248,7 @@
       </c>
       <c r="S23" s="10"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>2</v>
       </c>
@@ -1262,7 +1276,7 @@
       </c>
       <c r="S24" s="10"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
@@ -1288,7 +1302,7 @@
       </c>
       <c r="S25" s="5"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>2</v>
       </c>
@@ -1318,7 +1332,7 @@
       </c>
       <c r="S26" s="5"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1353,8 +1367,41 @@
         <v>2</v>
       </c>
       <c r="S27" s="10"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Z27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -1405,6 +1452,251 @@
       </c>
       <c r="Q28" t="s">
         <v>2</v>
+      </c>
+      <c r="Z28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ28" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="Z29" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG29" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ29" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AH30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI30" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AE31" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK31" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="Z32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ32" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="26:41" x14ac:dyDescent="0.2">
+      <c r="Z33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG33" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH33" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI33" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ33" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="26:41" x14ac:dyDescent="0.2">
+      <c r="AE34" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="26:41" x14ac:dyDescent="0.2">
+      <c r="AE35" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF35" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ35" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK35" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN35" t="s">
+        <v>6</v>
+      </c>
+      <c r="AO35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="26:41" x14ac:dyDescent="0.2">
+      <c r="AM36" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="26:41" x14ac:dyDescent="0.2">
+      <c r="AE37" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH37" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="26:41" x14ac:dyDescent="0.2">
+      <c r="AI38" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ38" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK38" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL38" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1414,10 +1706,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D931B7F0-D824-CF4B-A5DA-6DC9715A3593}">
-  <dimension ref="B1:AL55"/>
+  <dimension ref="B1:AL65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1812,6 +2104,12 @@
       <c r="I8" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="J8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="N8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1826,6 +2124,12 @@
       <c r="U8" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="X8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="Z8" s="4" t="s">
         <v>0</v>
       </c>
@@ -1875,6 +2179,12 @@
       </c>
       <c r="I9" s="6" t="s">
         <v>0</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>7</v>
@@ -1888,6 +2198,12 @@
         <v>7</v>
       </c>
       <c r="U9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="X9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y9" s="9" t="s">
         <v>7</v>
       </c>
       <c r="Z9" s="7" t="s">
@@ -2397,22 +2713,11 @@
     </row>
     <row r="23" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="T23" s="30"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
-      <c r="Y23" s="5"/>
-      <c r="Z23" s="5"/>
-      <c r="AA23" s="5"/>
-      <c r="AB23" s="5"/>
-      <c r="AC23" s="5"/>
-      <c r="AD23" s="5"/>
-      <c r="AE23" s="5"/>
-      <c r="AF23" s="5"/>
-      <c r="AG23" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="AH23" s="5"/>
       <c r="AI23" s="5"/>
       <c r="AJ23" s="5"/>
@@ -2420,20 +2725,6 @@
       <c r="AL23" s="5"/>
     </row>
     <row r="24" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
-      <c r="Y24" s="5"/>
-      <c r="Z24" s="5"/>
-      <c r="AA24" s="5"/>
-      <c r="AB24" s="5"/>
-      <c r="AC24" s="5"/>
-      <c r="AD24" s="5"/>
-      <c r="AE24" s="5"/>
-      <c r="AF24" s="5"/>
-      <c r="AG24" s="5"/>
       <c r="AH24" s="5"/>
       <c r="AI24" s="5"/>
       <c r="AJ24" s="5"/>
@@ -2441,32 +2732,50 @@
       <c r="AL24" s="5"/>
     </row>
     <row r="25" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="L25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
+      <c r="B25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="Z25" s="5"/>
       <c r="AA25" s="5"/>
-      <c r="AB25" s="5"/>
-      <c r="AC25" s="5"/>
-      <c r="AD25" s="5"/>
-      <c r="AE25" s="5"/>
-      <c r="AF25" s="5"/>
-      <c r="AG25" s="5"/>
+      <c r="AB25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="AH25" s="5"/>
       <c r="AI25" s="5"/>
       <c r="AJ25" s="5"/>
@@ -2474,382 +2783,440 @@
       <c r="AL25" s="5"/>
     </row>
     <row r="26" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="L26" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="P26" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
-      <c r="X26" s="5"/>
-      <c r="Y26" s="5"/>
+      <c r="B26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y26" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
-      <c r="AB26" s="5"/>
-      <c r="AC26" s="5"/>
-      <c r="AD26" s="5"/>
-      <c r="AE26" s="5"/>
-      <c r="AF26" s="5"/>
-      <c r="AG26" s="5"/>
-      <c r="AH26" s="5"/>
+      <c r="AB26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="AI26" s="5"/>
       <c r="AJ26" s="5"/>
       <c r="AK26" s="5"/>
       <c r="AL26" s="5"/>
     </row>
     <row r="27" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="L27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="T27" s="5"/>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
-      <c r="X27" s="5"/>
-      <c r="Y27" s="5"/>
-      <c r="Z27" s="5"/>
-      <c r="AA27" s="5"/>
-      <c r="AB27" s="5"/>
-      <c r="AC27" s="5"/>
-      <c r="AD27" s="5"/>
-      <c r="AE27" s="5"/>
-      <c r="AF27" s="5"/>
-      <c r="AG27" s="5"/>
-      <c r="AH27" s="5"/>
+      <c r="B27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="T27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="U27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="X27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="AI27" s="5"/>
       <c r="AJ27" s="5"/>
       <c r="AK27" s="5"/>
       <c r="AL27" s="5"/>
     </row>
     <row r="28" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="J28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O28" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
-      <c r="V28" s="5"/>
-      <c r="W28" s="5"/>
-      <c r="X28" s="5"/>
-      <c r="Y28" s="5"/>
-      <c r="Z28" s="5"/>
-      <c r="AA28" s="5"/>
-      <c r="AB28" s="5"/>
-      <c r="AC28" s="5"/>
-      <c r="AD28" s="5"/>
-      <c r="AE28" s="5"/>
-      <c r="AF28" s="5"/>
-      <c r="AG28" s="5"/>
-      <c r="AH28" s="5"/>
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="AI28" s="5"/>
       <c r="AJ28" s="5"/>
       <c r="AK28" s="5"/>
       <c r="AL28" s="5"/>
     </row>
     <row r="29" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
+      <c r="B29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="J29" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="L29" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="M29" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N29" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="O29" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
-      <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
-      <c r="AB29" s="5"/>
-      <c r="AC29" s="5"/>
-      <c r="AD29" s="5"/>
-      <c r="AE29" s="5"/>
-      <c r="AF29" s="5"/>
-      <c r="AG29" s="5"/>
-      <c r="AH29" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M29" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="V29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="AI29" s="5"/>
       <c r="AJ29" s="5"/>
       <c r="AK29" s="5"/>
       <c r="AL29" s="5"/>
     </row>
     <row r="30" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="C30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="T30" s="5"/>
-      <c r="U30" s="5"/>
-      <c r="V30" s="5"/>
-      <c r="W30" s="5"/>
-      <c r="X30" s="5"/>
-      <c r="Y30" s="5"/>
-      <c r="Z30" s="5"/>
-      <c r="AA30" s="5"/>
-      <c r="AB30" s="5"/>
-      <c r="AC30" s="5"/>
-      <c r="AD30" s="5"/>
-      <c r="AE30" s="5"/>
-      <c r="AF30" s="5"/>
-      <c r="AG30" s="5"/>
-      <c r="AH30" s="5"/>
+      <c r="J30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="V30" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="W30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y30" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="AI30" s="5"/>
       <c r="AJ30" s="5"/>
       <c r="AK30" s="5"/>
       <c r="AL30" s="5"/>
     </row>
     <row r="31" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="C31" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P31" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q31" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="5"/>
-      <c r="W31" s="5"/>
-      <c r="X31" s="5"/>
-      <c r="Y31" s="5"/>
-      <c r="Z31" s="5"/>
-      <c r="AA31" s="5"/>
-      <c r="AB31" s="5"/>
-      <c r="AC31" s="5"/>
-      <c r="AD31" s="5"/>
-      <c r="AE31" s="5"/>
-      <c r="AF31" s="5"/>
-      <c r="AG31" s="5"/>
-      <c r="AH31" s="5"/>
+      <c r="J31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O31" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE31" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="AI31" s="5"/>
       <c r="AJ31" s="5"/>
       <c r="AK31" s="5"/>
       <c r="AL31" s="5"/>
     </row>
     <row r="32" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="C32" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
-      <c r="X32" s="5"/>
-      <c r="Y32" s="5"/>
-      <c r="Z32" s="5"/>
-      <c r="AA32" s="5"/>
-      <c r="AB32" s="5"/>
-      <c r="AC32" s="5"/>
-      <c r="AD32" s="5"/>
-      <c r="AE32" s="5"/>
-      <c r="AF32" s="5"/>
-      <c r="AG32" s="5"/>
-      <c r="AH32" s="5"/>
+      <c r="T32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="U32" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="X32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y32" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB32" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE32" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="AI32" s="5"/>
       <c r="AJ32" s="5"/>
       <c r="AK32" s="5"/>
       <c r="AL32" s="5"/>
     </row>
     <row r="33" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="L33" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M33" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="T33" s="5"/>
-      <c r="U33" s="5"/>
-      <c r="V33" s="5"/>
-      <c r="W33" s="5"/>
-      <c r="X33" s="5"/>
-      <c r="Y33" s="5"/>
-      <c r="Z33" s="5"/>
-      <c r="AA33" s="5"/>
-      <c r="AB33" s="5"/>
-      <c r="AC33" s="5"/>
-      <c r="AD33" s="5"/>
-      <c r="AE33" s="5"/>
-      <c r="AF33" s="5"/>
-      <c r="AG33" s="5"/>
-      <c r="AH33" s="5"/>
       <c r="AI33" s="5"/>
       <c r="AJ33" s="5"/>
       <c r="AK33" s="5"/>
       <c r="AL33" s="5"/>
     </row>
     <row r="34" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="T34" s="5"/>
+      <c r="B34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="T34" s="30" t="s">
+        <v>55</v>
+      </c>
       <c r="U34" s="5"/>
       <c r="V34" s="5"/>
       <c r="W34" s="5"/>
@@ -2862,35 +3229,515 @@
       <c r="AD34" s="5"/>
       <c r="AE34" s="5"/>
       <c r="AF34" s="5"/>
-      <c r="AG34" s="5"/>
-      <c r="AH34" s="5"/>
       <c r="AI34" s="5"/>
       <c r="AJ34" s="5"/>
       <c r="AK34" s="5"/>
       <c r="AL34" s="5"/>
     </row>
+    <row r="35" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="5"/>
+      <c r="AB35" s="5"/>
+      <c r="AC35" s="5"/>
+      <c r="AD35" s="5"/>
+      <c r="AE35" s="5"/>
+      <c r="AF35" s="5"/>
+    </row>
+    <row r="36" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="K36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE36" s="5"/>
+      <c r="AF36" s="5"/>
+    </row>
+    <row r="37" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="K37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L37" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="O37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P37" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="T37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="V37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC37" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD37" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE37" s="5"/>
+      <c r="AF37" s="5"/>
+    </row>
+    <row r="38" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="K38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T38" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U38" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="V38" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W38" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="X38" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG38" s="5"/>
+    </row>
+    <row r="39" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="I39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC39" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD39" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG39" s="5"/>
+    </row>
+    <row r="40" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M40" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N40" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="5"/>
+      <c r="W40" s="5"/>
+      <c r="X40" s="5"/>
+      <c r="Y40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG40" s="5"/>
+    </row>
+    <row r="41" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE41" s="5"/>
+      <c r="AF41" s="5"/>
+    </row>
+    <row r="42" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="B42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P42" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="5"/>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB42" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC42" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD42" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE42" s="5"/>
+      <c r="AF42" s="5"/>
+    </row>
+    <row r="43" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="B43" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="T43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="5"/>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA43" s="5"/>
+      <c r="AB43" s="5"/>
+      <c r="AC43" s="5"/>
+      <c r="AD43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE43" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L44" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="5"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z44" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA44" s="5"/>
+      <c r="AB44" s="5"/>
+      <c r="AC44" s="5"/>
+      <c r="AD44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE44" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="47" spans="2:38" x14ac:dyDescent="0.2">
       <c r="AI47" s="5"/>
     </row>
     <row r="48" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B48" s="5"/>
       <c r="AI48" s="5"/>
     </row>
     <row r="49" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B49" s="5"/>
       <c r="AI49" s="5"/>
     </row>
-    <row r="50" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B50" s="5"/>
-    </row>
-    <row r="51" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B51" s="5"/>
-    </row>
-    <row r="54" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="Z54" s="5"/>
-    </row>
-    <row r="55" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="X55" s="5"/>
+    <row r="63" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B63" s="5"/>
+    </row>
+    <row r="64" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="B64" s="5"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2902,7 +3749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90DFA3C2-026B-9A43-980D-E8D28F7CC247}">
   <dimension ref="B1:AG183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
In PvT anti-rush, build a cannon closer to the start block
</commit_message>
<xml_diff>
--- a/docs/Blocks.xlsx
+++ b/docs/Blocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmnielsen/BW/Stardust/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59973DB-5505-BB45-AA09-D36DDFAC1580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A0DF1E-25ED-AB45-905A-4E389D755C16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="460" windowWidth="31260" windowHeight="20540" xr2:uid="{A8F001C3-164F-CB44-AE85-D1EDAAFCF585}"/>
+    <workbookView xWindow="1120" yWindow="460" windowWidth="31260" windowHeight="20540" activeTab="1" xr2:uid="{A8F001C3-164F-CB44-AE85-D1EDAAFCF585}"/>
   </bookViews>
   <sheets>
     <sheet name="Power" sheetId="2" r:id="rId1"/>
@@ -700,7 +700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0F9ED0-5771-1442-9F18-E1B361EBF084}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1425,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D931B7F0-D824-CF4B-A5DA-6DC9715A3593}">
   <dimension ref="B1:AL65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB25" sqref="AB25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AE35" sqref="AE35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1619,10 +1619,10 @@
       <c r="Y5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Z5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="3" t="s">
+      <c r="Z5" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="24" t="s">
         <v>1</v>
       </c>
       <c r="AB5" s="1" t="s">
@@ -1663,10 +1663,10 @@
       <c r="G6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="H6" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="24" t="s">
         <v>1</v>
       </c>
       <c r="J6" s="4" t="s">
@@ -1695,10 +1695,10 @@
       <c r="Y6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Z6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="9" t="s">
+      <c r="Z6" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="26" t="s">
         <v>1</v>
       </c>
       <c r="AB6" s="4" t="s">
@@ -1739,10 +1739,10 @@
       <c r="G7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="9" t="s">
+      <c r="H7" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="26" t="s">
         <v>1</v>
       </c>
       <c r="J7" s="7" t="s">
@@ -2134,10 +2134,10 @@
       <c r="D17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="E17" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="24" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -2164,10 +2164,10 @@
       <c r="Y17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Z17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA17" s="3" t="s">
+      <c r="Z17" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="24" t="s">
         <v>1</v>
       </c>
       <c r="AB17" s="1" t="s">
@@ -2190,10 +2190,10 @@
       <c r="D18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="9" t="s">
+      <c r="E18" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="26" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
@@ -2220,10 +2220,10 @@
       <c r="Y18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="Z18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA18" s="9" t="s">
+      <c r="Z18" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="26" t="s">
         <v>1</v>
       </c>
       <c r="AB18" s="7" t="s">
@@ -2664,10 +2664,10 @@
       <c r="G28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" s="3" t="s">
+      <c r="H28" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="24" t="s">
         <v>1</v>
       </c>
       <c r="J28" s="4" t="s">
@@ -2736,10 +2736,10 @@
       <c r="G29" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="9" t="s">
+      <c r="H29" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="26" t="s">
         <v>1</v>
       </c>
       <c r="J29" s="7" t="s">
@@ -2766,10 +2766,10 @@
       <c r="Y29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Z29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA29" s="3" t="s">
+      <c r="Z29" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="24" t="s">
         <v>1</v>
       </c>
       <c r="AB29" s="4" t="s">
@@ -2814,10 +2814,10 @@
       <c r="Y30" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="Z30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA30" s="9" t="s">
+      <c r="Z30" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="26" t="s">
         <v>1</v>
       </c>
       <c r="AB30" s="7" t="s">
@@ -3125,10 +3125,10 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
-      <c r="I39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J39" s="3" t="s">
+      <c r="I39" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39" s="24" t="s">
         <v>1</v>
       </c>
       <c r="K39" s="4" t="s">
@@ -3168,10 +3168,10 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
-      <c r="I40" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J40" s="9" t="s">
+      <c r="I40" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="J40" s="26" t="s">
         <v>1</v>
       </c>
       <c r="K40" s="7" t="s">
@@ -3191,10 +3191,10 @@
       <c r="V40" s="5"/>
       <c r="W40" s="5"/>
       <c r="X40" s="5"/>
-      <c r="Y40" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z40" s="3" t="s">
+      <c r="Y40" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="24" t="s">
         <v>1</v>
       </c>
       <c r="AA40" s="1" t="s">
@@ -3262,10 +3262,10 @@
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
       <c r="X41" s="5"/>
-      <c r="Y41" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z41" s="9" t="s">
+      <c r="Y41" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="26" t="s">
         <v>1</v>
       </c>
       <c r="AA41" s="4" t="s">

</xml_diff>

<commit_message>
Add new start blocks for Outsider
</commit_message>
<xml_diff>
--- a/docs/Blocks.xlsx
+++ b/docs/Blocks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmnielsen/BW/Stardust/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A0DF1E-25ED-AB45-905A-4E389D755C16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EC07BC-C354-6C42-B714-1FF88A71C903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="460" windowWidth="31260" windowHeight="20540" activeTab="1" xr2:uid="{A8F001C3-164F-CB44-AE85-D1EDAAFCF585}"/>
+    <workbookView xWindow="1120" yWindow="500" windowWidth="31260" windowHeight="20540" activeTab="1" xr2:uid="{A8F001C3-164F-CB44-AE85-D1EDAAFCF585}"/>
   </bookViews>
   <sheets>
     <sheet name="Power" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="59">
   <si>
     <t>L</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>Right of nexus, vertical</t>
+  </si>
+  <si>
+    <t>Left of nexus, above and below</t>
+  </si>
+  <si>
+    <t>Below nexus</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -700,7 +706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0F9ED0-5771-1442-9F18-E1B361EBF084}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1418,6 +1426,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Classification: Public</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1425,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D931B7F0-D824-CF4B-A5DA-6DC9715A3593}">
   <dimension ref="B1:AL65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE35" sqref="AE35"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3438,19 +3449,536 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="AI47" s="5"/>
+    <row r="46" spans="2:38" x14ac:dyDescent="0.2">
+      <c r="B46" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="T46" s="11" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="48" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="AI48" s="5"/>
-    </row>
-    <row r="49" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="AI49" s="5"/>
-    </row>
-    <row r="63" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="J48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="X48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD48" s="5"/>
+      <c r="AE48" s="5"/>
+    </row>
+    <row r="49" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="J49" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L49" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M49" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N49" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="O49" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
+      <c r="V49" s="5"/>
+      <c r="X49" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y49" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z49" s="5"/>
+      <c r="AA49" s="5"/>
+      <c r="AB49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC49" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD49" s="5"/>
+      <c r="AE49" s="5"/>
+    </row>
+    <row r="50" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="L50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q50" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+      <c r="V50" s="5"/>
+      <c r="Z50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC50" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="T51" s="5"/>
+      <c r="U51" s="5"/>
+      <c r="V51" s="5"/>
+      <c r="X51" s="30"/>
+      <c r="Y51" s="30"/>
+      <c r="Z51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE51" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K52" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="L52" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M52" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N52" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="O52" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q52" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T52" s="5"/>
+      <c r="U52" s="5"/>
+      <c r="V52" s="5"/>
+      <c r="W52" s="5"/>
+      <c r="X52" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y52" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z52" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA52" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB52" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC52" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD52" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE52" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="K53" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="L53" s="2"/>
+      <c r="M53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q53" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y53" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA53" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE53" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF53" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG53" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N54" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="T54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="X54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z54" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC54" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD54" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG54" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B55" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="T55" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U55" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="V55" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="W55" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X55" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y55" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z55" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA55" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB55" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC55" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD55" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE55" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF55" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG55" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B56" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="5"/>
+      <c r="V56" s="5"/>
+      <c r="W56" s="5"/>
+      <c r="X56" s="5"/>
+      <c r="Y56" s="5"/>
+      <c r="Z56" s="5"/>
+      <c r="AA56" s="5"/>
+      <c r="AB56" s="5"/>
+      <c r="AC56" s="5"/>
+      <c r="AD56" s="5"/>
+      <c r="AE56" s="5"/>
+      <c r="AF56" s="5"/>
+      <c r="AG56" s="5"/>
+      <c r="AH56" s="5"/>
+    </row>
+    <row r="57" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="X57" s="5"/>
+      <c r="Y57" s="5"/>
+      <c r="Z57" s="5"/>
+      <c r="AA57" s="5"/>
+      <c r="AB57" s="5"/>
+      <c r="AC57" s="5"/>
+      <c r="AD57" s="5"/>
+      <c r="AE57" s="5"/>
+      <c r="AF57" s="5"/>
+      <c r="AG57" s="5"/>
+      <c r="AH57" s="5"/>
+    </row>
+    <row r="58" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="X58" s="5"/>
+      <c r="Y58" s="5"/>
+      <c r="Z58" s="5"/>
+      <c r="AA58" s="5"/>
+      <c r="AB58" s="5"/>
+      <c r="AC58" s="5"/>
+      <c r="AD58" s="5"/>
+      <c r="AE58" s="5"/>
+      <c r="AF58" s="5"/>
+      <c r="AG58" s="5"/>
+      <c r="AH58" s="5"/>
+    </row>
+    <row r="63" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B63" s="5"/>
     </row>
-    <row r="64" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B64" s="5"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
@@ -3459,6 +3987,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Classification: Public</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -7827,5 +8358,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Classification: Public</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>